<commit_message>
Reformat text for initial sprint backlog
</commit_message>
<xml_diff>
--- a/Project2/sprint_backlogs/Initial_Sprint_Backlog.xlsx
+++ b/Project2/sprint_backlogs/Initial_Sprint_Backlog.xlsx
@@ -24,8 +24,22 @@
 So that I can bring in different files from different balloting locations.</t>
   </si>
   <si>
-    <t xml:space="preserve">Bring in file names from command line
-Bring in file names from directory if no filename arguments </t>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+        <sz val="12.0"/>
+      </rPr>
+      <t>Bring in file names from command line
+Bring in file names from directory if no filename arguments</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
   </si>
   <si>
     <t>Acceptance Criteria:
@@ -207,7 +221,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -216,6 +230,7 @@
     </font>
     <font>
       <b/>
+      <sz val="20.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -226,6 +241,12 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -259,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -269,12 +290,13 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -493,7 +515,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="8.0"/>
     <col customWidth="1" min="2" max="2" width="36.13"/>
-    <col customWidth="1" min="4" max="4" width="38.0"/>
+    <col customWidth="1" min="4" max="4" width="53.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -592,6 +614,7 @@
       <c r="B20" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="C20" s="5"/>
       <c r="D20" s="4" t="s">
         <v>9</v>
       </c>
@@ -600,26 +623,39 @@
       <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22">
       <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23">
       <c r="B23" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24">
       <c r="B24" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25">
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26">
       <c r="B26" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="4" t="s">
         <v>18</v>
       </c>
@@ -628,26 +664,39 @@
       <c r="B27" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28">
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29">
       <c r="B29" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30">
       <c r="B30" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31">
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32">
       <c r="B32" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="C32" s="5"/>
       <c r="D32" s="4" t="s">
         <v>21</v>
       </c>
@@ -656,26 +705,39 @@
       <c r="B33" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34">
       <c r="B34" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35">
       <c r="B35" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36">
       <c r="B36" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37">
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38">
       <c r="B38" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="C38" s="5"/>
       <c r="D38" s="4" t="s">
         <v>26</v>
       </c>
@@ -684,26 +746,39 @@
       <c r="B39" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40">
       <c r="B40" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41">
       <c r="B41" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="42">
       <c r="B42" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43">
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44">
       <c r="B44" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="C44" s="5"/>
       <c r="D44" s="4" t="s">
         <v>29</v>
       </c>
@@ -712,26 +787,39 @@
       <c r="B45" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
     </row>
     <row r="46">
       <c r="B46" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47">
       <c r="B47" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
     </row>
     <row r="48">
       <c r="B48" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+    </row>
+    <row r="49">
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
     </row>
     <row r="50">
       <c r="B50" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="C50" s="5"/>
       <c r="D50" s="4" t="s">
         <v>9</v>
       </c>
@@ -740,26 +828,39 @@
       <c r="B51" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
     </row>
     <row r="52">
       <c r="B52" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
     </row>
     <row r="53">
       <c r="B53" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
     </row>
     <row r="54">
       <c r="B54" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55">
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
     </row>
     <row r="56">
       <c r="B56" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="C56" s="5"/>
       <c r="D56" s="4" t="s">
         <v>13</v>
       </c>
@@ -768,26 +869,39 @@
       <c r="B57" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
     </row>
     <row r="58">
       <c r="B58" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
     </row>
     <row r="59">
       <c r="B59" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
     </row>
     <row r="60">
       <c r="B60" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+    </row>
+    <row r="61">
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
     </row>
     <row r="62">
       <c r="B62" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="C62" s="5"/>
       <c r="D62" s="4" t="s">
         <v>36</v>
       </c>
@@ -796,26 +910,39 @@
       <c r="B63" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
     </row>
     <row r="64">
       <c r="B64" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
     </row>
     <row r="65">
       <c r="B65" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
     </row>
     <row r="66">
       <c r="B66" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67">
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
     </row>
     <row r="68">
       <c r="B68" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="C68" s="5"/>
       <c r="D68" s="4" t="s">
         <v>40</v>
       </c>
@@ -824,26 +951,39 @@
       <c r="B69" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
     </row>
     <row r="70">
       <c r="B70" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
     </row>
     <row r="71">
       <c r="B71" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
     </row>
     <row r="72">
       <c r="B72" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73">
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
     </row>
     <row r="74">
       <c r="B74" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="C74" s="5"/>
       <c r="D74" s="4" t="s">
         <v>43</v>
       </c>
@@ -852,21 +992,37 @@
       <c r="B75" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
     </row>
     <row r="76">
       <c r="B76" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
     </row>
     <row r="77">
       <c r="B77" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
     </row>
     <row r="78">
       <c r="B78" s="2" t="s">
         <v>38</v>
       </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+    </row>
+    <row r="79">
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80">
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>